<commit_message>
code till seventeen july competition task
</commit_message>
<xml_diff>
--- a/Mars Automation Solution/Mars Competition Task/TestData/TestData.xlsx
+++ b/Mars Automation Solution/Mars Competition Task/TestData/TestData.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mvpstudio\vscode\repos\mvpstudio\Mars Automation Solution\Mars Competition Task\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2BF79A1-1CDB-4F0E-A2BA-13E3AEBA40D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C555F4B3-0C60-4A79-B82B-D86ACF5D57E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignIn" sheetId="1" r:id="rId1"/>
     <sheet name="ShareSkill" sheetId="2" r:id="rId2"/>
+    <sheet name="ManageListing" sheetId="3" r:id="rId3"/>
+    <sheet name="ServiceDetail" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>url</t>
   </si>
@@ -109,9 +111,6 @@
     <t>Hidden</t>
   </si>
   <si>
-    <t>aaaa cccc</t>
-  </si>
-  <si>
     <t>cccc cccc</t>
   </si>
   <si>
@@ -119,6 +118,48 @@
   </si>
   <si>
     <t>Marketing</t>
+  </si>
+  <si>
+    <t>Title editted</t>
+  </si>
+  <si>
+    <t>http://192.168.99.100:5000/Home/ServiceListing/?id=60d82811b4b34c00014c766a</t>
+  </si>
+  <si>
+    <t>Deleteaction</t>
+  </si>
+  <si>
+    <t>Selenium</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Chatboxvalues</t>
+  </si>
+  <si>
+    <t>Hi How are you?</t>
+  </si>
+  <si>
+    <t>http://192.168.99.100:5000/Home/ServiceDetail?id=60d460539b4eae0001de9f70</t>
+  </si>
+  <si>
+    <t>Description editted</t>
+  </si>
+  <si>
+    <t>Title is Entered</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Subcategory</t>
+  </si>
+  <si>
+    <t>Graphics &amp; Design</t>
+  </si>
+  <si>
+    <t>Book &amp; Album covers</t>
   </si>
 </sst>
 </file>
@@ -510,9 +551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -555,10 +594,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575782E1-9A84-46B6-94EF-B230E0AAB0E1}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -571,9 +610,11 @@
     <col min="7" max="7" width="17.21875" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
     <col min="12" max="12" width="18.88671875" customWidth="1"/>
+    <col min="15" max="15" width="18.5546875" customWidth="1"/>
+    <col min="16" max="16" width="30.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -581,7 +622,7 @@
         <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>8</v>
@@ -616,16 +657,22 @@
       <c r="N1" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="O1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
@@ -659,9 +706,106 @@
       </c>
       <c r="N2" s="2" t="s">
         <v>23</v>
+      </c>
+      <c r="O2" t="s">
+        <v>39</v>
+      </c>
+      <c r="P2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D411794-51ED-4287-98D3-9F6C30D943F5}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="69.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="27.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{3AC53E40-5B40-47E2-B15A-4CE7F1A75FC2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9B23DF0-CEA9-44F5-BC2A-1F18F4CBE0F3}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.44140625" customWidth="1"/>
+    <col min="2" max="2" width="70.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{10E8115A-6163-414A-8BE4-96DF081118FE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Competition_Task 1 and Task 2 Submission
</commit_message>
<xml_diff>
--- a/Mars Automation Solution/Mars Competition Task/TestData/TestData.xlsx
+++ b/Mars Automation Solution/Mars Competition Task/TestData/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mvpstudio\vscode\repos\mvpstudio\Mars Automation Solution\Mars Competition Task\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C555F4B3-0C60-4A79-B82B-D86ACF5D57E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7519A58C-1AD6-4E66-9F78-3D732F68B692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignIn" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
   <si>
     <t>url</t>
   </si>
@@ -69,12 +69,6 @@
     <t>LocationType</t>
   </si>
   <si>
-    <t>Startdate</t>
-  </si>
-  <si>
-    <t>Enddate</t>
-  </si>
-  <si>
     <t>Selectday</t>
   </si>
   <si>
@@ -108,69 +102,95 @@
     <t>Performance Testing</t>
   </si>
   <si>
+    <t>cccc cccc</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Title editted</t>
+  </si>
+  <si>
+    <t>Deleteaction</t>
+  </si>
+  <si>
+    <t>Selenium</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Chatboxvalues</t>
+  </si>
+  <si>
+    <t>Hi How are you?</t>
+  </si>
+  <si>
+    <t>Description editted</t>
+  </si>
+  <si>
+    <t>Title is Entered</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Subcategory</t>
+  </si>
+  <si>
+    <t>Graphics &amp; Design</t>
+  </si>
+  <si>
+    <t>Book &amp; Album covers</t>
+  </si>
+  <si>
+    <t>AddDaysInCurrentDateToStart</t>
+  </si>
+  <si>
+    <t>AddDaysInCurrentDateToEnd</t>
+  </si>
+  <si>
+    <t>http://192.168.99.100:5000/Home/ServiceDetail</t>
+  </si>
+  <si>
+    <t>http://192.168.99.100:5000/Home/ServiceListing</t>
+  </si>
+  <si>
+    <t>Creditvalue</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Mon,Wed,Fri</t>
+  </si>
+  <si>
+    <t>10:00,10:00,10:00</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>11:00,11:00,11:00</t>
+  </si>
+  <si>
+    <t>Online</t>
+  </si>
+  <si>
     <t>Hidden</t>
-  </si>
-  <si>
-    <t>cccc cccc</t>
-  </si>
-  <si>
-    <t>Tag</t>
-  </si>
-  <si>
-    <t>Marketing</t>
-  </si>
-  <si>
-    <t>Title editted</t>
-  </si>
-  <si>
-    <t>http://192.168.99.100:5000/Home/ServiceListing/?id=60d82811b4b34c00014c766a</t>
-  </si>
-  <si>
-    <t>Deleteaction</t>
-  </si>
-  <si>
-    <t>Selenium</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Chatboxvalues</t>
-  </si>
-  <si>
-    <t>Hi How are you?</t>
-  </si>
-  <si>
-    <t>http://192.168.99.100:5000/Home/ServiceDetail?id=60d460539b4eae0001de9f70</t>
-  </si>
-  <si>
-    <t>Description editted</t>
-  </si>
-  <si>
-    <t>Title is Entered</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Subcategory</t>
-  </si>
-  <si>
-    <t>Graphics &amp; Design</t>
-  </si>
-  <si>
-    <t>Book &amp; Album covers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
-    <numFmt numFmtId="165" formatCode="hh:mm:ss;@"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,6 +213,21 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -203,7 +238,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -217,27 +252,41 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="2" xr:uid="{4BC69256-0A69-46A8-A5B8-A9DB1D7B1300}"/>
+    <cellStyle name="Hyperlink 2 2" xfId="4" xr:uid="{7C3B5EF8-AC8C-4793-A234-FC2B353F0550}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{8DAAF0C8-156D-4CED-BCA0-20BEC117D498}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -551,7 +600,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -561,13 +612,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -594,10 +645,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575782E1-9A84-46B6-94EF-B230E0AAB0E1}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -606,133 +657,165 @@
     <col min="2" max="3" width="20.21875" style="2" customWidth="1"/>
     <col min="4" max="4" width="19.109375" customWidth="1"/>
     <col min="5" max="5" width="16.77734375" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" customWidth="1"/>
-    <col min="7" max="7" width="17.21875" customWidth="1"/>
-    <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="12" max="12" width="18.88671875" customWidth="1"/>
-    <col min="15" max="15" width="18.5546875" customWidth="1"/>
-    <col min="16" max="16" width="30.77734375" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="2"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="18.88671875" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="18.5546875" customWidth="1"/>
+    <col min="15" max="15" width="30.77734375" customWidth="1"/>
+    <col min="16" max="16" width="14.6640625" customWidth="1"/>
+    <col min="17" max="17" width="17.109375" customWidth="1"/>
+    <col min="18" max="18" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="F2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="2">
+        <v>10</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="5">
-        <v>43567</v>
-      </c>
-      <c r="G2" s="4">
-        <v>43597</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="J2" s="6">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" t="s">
-        <v>39</v>
-      </c>
-      <c r="P2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>35</v>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="R2" r:id="rId1" xr:uid="{01748E69-D947-48D7-BFD0-710361277914}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D411794-51ED-4287-98D3-9F6C30D943F5}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -743,25 +826,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>29</v>
+      <c r="C1" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -776,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9B23DF0-CEA9-44F5-BC2A-1F18F4CBE0F3}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -787,19 +875,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hi Salani, Competition task submission with suggested modifications
</commit_message>
<xml_diff>
--- a/Mars Automation Solution/Mars Competition Task/TestData/TestData.xlsx
+++ b/Mars Automation Solution/Mars Competition Task/TestData/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mvpstudio\vscode\repos\mvpstudio\Mars Automation Solution\Mars Competition Task\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7519A58C-1AD6-4E66-9F78-3D732F68B692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC32B66-01CA-4F42-BA3D-7F7907A8A3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3168" yWindow="3168" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignIn" sheetId="1" r:id="rId1"/>
@@ -647,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575782E1-9A84-46B6-94EF-B230E0AAB0E1}">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -864,7 +864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9B23DF0-CEA9-44F5-BC2A-1F18F4CBE0F3}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>